<commit_message>
fixed inaccuracies in dataset
</commit_message>
<xml_diff>
--- a/server/data/output.xlsx
+++ b/server/data/output.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="O:\Projects\NumericalReference\server\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC3D9EFE-74DE-4E9A-A05C-A774232ED1D1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F2A5D0-AC53-4732-8453-81F6D2390DED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" tabRatio="348" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -334,24 +334,15 @@
     <t>the energy generated by consuming an apple</t>
   </si>
   <si>
-    <t>397.5 J</t>
-  </si>
-  <si>
     <t>https://fdc.nal.usda.gov/</t>
   </si>
   <si>
     <t>the energy generated by consuming a banana</t>
   </si>
   <si>
-    <t>439.3 J</t>
-  </si>
-  <si>
     <t>the energy generated by consuming a slice of bread</t>
   </si>
   <si>
-    <t>343.1 J</t>
-  </si>
-  <si>
     <t>the energy released by the Sun every second</t>
   </si>
   <si>
@@ -1015,9 +1006,6 @@
     <t>the weight of one litre of water</t>
   </si>
   <si>
-    <t>the kinetic energy of a punch</t>
-  </si>
-  <si>
     <t>275 J</t>
   </si>
   <si>
@@ -1223,6 +1211,18 @@
   </si>
   <si>
     <t>1.60934 km</t>
+  </si>
+  <si>
+    <t>54 kcal</t>
+  </si>
+  <si>
+    <t>76 kcal</t>
+  </si>
+  <si>
+    <t>112 kcal</t>
+  </si>
+  <si>
+    <t>the kinetic energy of a punch (by a human)</t>
   </si>
 </sst>
 </file>
@@ -1620,8 +1620,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C152"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A60" sqref="A60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1633,7 +1633,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -1728,7 +1728,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>24</v>
@@ -1739,7 +1739,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>26</v>
@@ -1750,10 +1750,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>30</v>
@@ -1761,24 +1761,24 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="B13" s="3">
         <v>3116480</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1788,7 +1788,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1839,13 +1839,13 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -2026,13 +2026,13 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
@@ -2048,24 +2048,24 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
@@ -2075,7 +2075,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2140,175 +2140,175 @@
         <v>103</v>
       </c>
       <c r="B49" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>107</v>
+        <v>399</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>109</v>
+        <v>398</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>331</v>
+        <v>400</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>341</v>
+        <v>337</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
@@ -2318,17 +2318,17 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>86</v>
@@ -2336,208 +2336,208 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>39</v>
@@ -2545,21 +2545,21 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>33</v>
@@ -2567,10 +2567,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>30</v>
@@ -2578,90 +2578,90 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2671,363 +2671,363 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B104" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="C104" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C112" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="C118" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C119" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="C120" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C121" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="B126" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C126" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="B127" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C127" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B128" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C128" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B129" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C129" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="B130" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C130" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="B133" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C133" t="s">
         <v>39</v>
@@ -3035,10 +3035,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="B134" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C134" t="s">
         <v>39</v>
@@ -3046,54 +3046,54 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="B135" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C135" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B136" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C136" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="B137" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C137" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="B138" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C138" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B139" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="C139" s="1" t="s">
         <v>80</v>
@@ -3101,87 +3101,87 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="B140" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="C140" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="B141" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="C141" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="B142" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C142" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="B143" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C143" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B144" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C144" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="B145" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="C145" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="B146" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C146" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="B147" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C147" t="s">
         <v>33</v>
@@ -3189,10 +3189,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="B148" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C148" t="s">
         <v>39</v>
@@ -3200,10 +3200,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="B149" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="C149" t="s">
         <v>36</v>
@@ -3211,24 +3211,24 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="B150" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="C150" s="1" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="B151" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="C151" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>